<commit_message>
[Add] Download file template nilasi seleksi
</commit_message>
<xml_diff>
--- a/cypress/downloads/template_import_nilai_pendaftar.xlsx
+++ b/cypress/downloads/template_import_nilai_pendaftar.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="645" windowWidth="19815" windowHeight="8640"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Format Inputan" sheetId="1" r:id="rId1"/>
+    <sheet name="Format Inputan" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>ID Pendaftar</t>
   </si>
@@ -61,9 +62,6 @@
     <t>90.00</t>
   </si>
   <si>
-    <t>v</t>
-  </si>
-  <si>
     <t>selamat</t>
   </si>
   <si>
@@ -103,6 +101,9 @@
     <t>TEST123</t>
   </si>
   <si>
+    <t>0.00</t>
+  </si>
+  <si>
     <t>123000067</t>
   </si>
   <si>
@@ -221,26 +222,28 @@
   </si>
   <si>
     <t>IGA MASARDI</t>
-  </si>
-  <si>
-    <t>88.00</t>
-  </si>
-  <si>
-    <t>Lulus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -251,38 +254,34 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf xfId="0" fontId="0" numFmtId="49" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -572,24 +571,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="29.421387" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="50.559082" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="22.280273" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -622,14 +625,16 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
+      <c r="D2"/>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -639,51 +644,60 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
+      <c r="D3"/>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4"/>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
+      <c r="D6"/>
       <c r="E6" t="s">
         <v>14</v>
       </c>
@@ -691,30 +705,29 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7"/>
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" t="s">
-        <v>69</v>
-      </c>
       <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -724,14 +737,16 @@
       <c r="C8" t="s">
         <v>31</v>
       </c>
+      <c r="D8"/>
       <c r="E8" t="s">
         <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -741,14 +756,16 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
+      <c r="D9"/>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -758,55 +775,76 @@
       <c r="C10" t="s">
         <v>38</v>
       </c>
+      <c r="D10"/>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
       <c r="F10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>39</v>
       </c>
+      <c r="B11"/>
       <c r="C11" t="s">
         <v>40</v>
       </c>
+      <c r="D11"/>
+      <c r="E11"/>
       <c r="F11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>41</v>
       </c>
+      <c r="B12"/>
       <c r="C12" t="s">
         <v>42</v>
       </c>
+      <c r="D12"/>
+      <c r="E12"/>
       <c r="F12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>43</v>
       </c>
+      <c r="B13"/>
       <c r="C13" t="s">
         <v>44</v>
       </c>
+      <c r="D13"/>
+      <c r="E13"/>
       <c r="F13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>45</v>
       </c>
+      <c r="B14"/>
       <c r="C14" t="s">
         <v>46</v>
       </c>
+      <c r="D14"/>
+      <c r="E14"/>
       <c r="F14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -816,22 +854,29 @@
       <c r="C15" t="s">
         <v>49</v>
       </c>
+      <c r="D15"/>
+      <c r="E15"/>
       <c r="F15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>50</v>
       </c>
+      <c r="B16"/>
       <c r="C16" t="s">
         <v>51</v>
       </c>
+      <c r="D16"/>
+      <c r="E16"/>
       <c r="F16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -841,22 +886,29 @@
       <c r="C17" t="s">
         <v>54</v>
       </c>
+      <c r="D17"/>
+      <c r="E17"/>
       <c r="F17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>55</v>
       </c>
+      <c r="B18"/>
       <c r="C18" t="s">
         <v>56</v>
       </c>
+      <c r="D18"/>
+      <c r="E18"/>
       <c r="F18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -866,22 +918,29 @@
       <c r="C19" t="s">
         <v>59</v>
       </c>
+      <c r="D19"/>
+      <c r="E19"/>
       <c r="F19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>60</v>
       </c>
+      <c r="B20"/>
       <c r="C20" t="s">
         <v>61</v>
       </c>
+      <c r="D20"/>
+      <c r="E20"/>
       <c r="F20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -891,34 +950,57 @@
       <c r="C21" t="s">
         <v>64</v>
       </c>
+      <c r="D21"/>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
       <c r="F21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>65</v>
       </c>
+      <c r="B22"/>
       <c r="C22" t="s">
         <v>66</v>
       </c>
+      <c r="D22"/>
+      <c r="E22"/>
       <c r="F22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>67</v>
       </c>
+      <c r="B23"/>
       <c r="C23" t="s">
         <v>68</v>
       </c>
+      <c r="D23"/>
+      <c r="E23"/>
       <c r="F23" t="s">
         <v>10</v>
       </c>
+      <c r="G23"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>